<commit_message>
Pedido de restituição completo
Faltando apenas o front e o envio e assinatura, porém é necessário testar em uma empresa liberada e pronta para solicitar os pedidos!
</commit_message>
<xml_diff>
--- a/comp.xlsx
+++ b/comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lima\Desktop\Python geral\rpa-pedido-restituicao-ECAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A1487-7F57-46B6-BCF9-05E5C72C1A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44202214-FEB2-4C9E-882F-45B7774A42F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CCEEF96-4F95-46B1-9813-034BBBAC59EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>1138-01</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>497,40</t>
+  </si>
+  <si>
+    <t>1200,00</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +632,8 @@
       <c r="E2" s="4">
         <v>112.33</v>
       </c>
-      <c r="F2" s="4">
-        <v>8.98</v>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="G2" s="4">
         <v>44.93</v>

</xml_diff>